<commit_message>
Updated the AML_Tuning notebook and AML Tuning presentation
</commit_message>
<xml_diff>
--- a/my_excel.xlsx
+++ b/my_excel.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gangu\OneDrive\Desktop\Academics\Rule Based Statistical Approach for AML Threshold Tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B8DB7-D26E-4396-81F9-E20912809FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077D0625-4F45-4073-AEA5-7228BA2726F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -636,14 +647,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="W10:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="10" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W10">
+        <f>472/(3128+1861+472+539)</f>
+        <v>7.8666666666666663E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="23:23" x14ac:dyDescent="0.3">
+      <c r="W25">
+        <f>281/(2069+1257+281+393)</f>
+        <v>7.0250000000000007E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>